<commit_message>
Eerste update code en passend maken Excels
</commit_message>
<xml_diff>
--- a/Bus Planning.xlsx
+++ b/Bus Planning.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stichtingfontys-my.sharepoint.com/personal/872575_fontys_nl/Documents/Documenten/Python/PJ5 Dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/54fb42b29621d9c9/Documents/Project 5 kans 2/GithubCode/Project_5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_0399E22E9067360E62355476585DCE3A87431D38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE366500-D517-4BCD-A4AF-9BBB621D2634}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="11_0399E22E9067360E62355476585DCE3A87431D38" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AE1DCEB-7C00-4F4E-B478-C2EFF5967663}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4512" yWindow="2616" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2009,6 +2009,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2360,6 +2361,15 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -19935,6 +19945,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010013B620F01982514694878B55267266B0" ma:contentTypeVersion="85" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="f20b580f4bc73672f7fc26b54f2fdd7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="882bdec5-c3ce-4705-9a84-58ed8ad203ea" xmlns:ns3="c6fe3531-949f-4c96-ac1d-b793c48e3f25" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9324efb3ca4fd789e46a4cfe415928a3" ns2:_="" ns3:_="">
     <xsd:import namespace="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
@@ -20155,15 +20174,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -20173,13 +20183,38 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C21D0A-65D6-47B6-8E76-5D8CAE45D404}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C58A68F-A5E9-4F6F-AD01-06B5D5C01F66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C58A68F-A5E9-4F6F-AD01-06B5D5C01F66}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{53C21D0A-65D6-47B6-8E76-5D8CAE45D404}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
+    <ds:schemaRef ds:uri="c6fe3531-949f-4c96-ac1d-b793c48e3f25"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABD986A7-2A39-40F9-A024-B808D196BF4D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ABD986A7-2A39-40F9-A024-B808D196BF4D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="882bdec5-c3ce-4705-9a84-58ed8ad203ea"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>